<commit_message>
use ngsi-ld context names for core elements
</commit_message>
<xml_diff>
--- a/models/jsonld/redundancies-identified-and-removed.xlsx
+++ b/models/jsonld/redundancies-identified-and-removed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rap/GitRepositories/GitHub/DEMETER/models/jsonld/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CE64A3-6CB4-CC44-8F86-A121457B407A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F61928-88E2-F44D-AD3D-56B00450F509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="2960" windowWidth="26040" windowHeight="14540" xr2:uid="{4E7EF15A-308C-654F-BE72-EC858B7BEAD8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4026" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4030" uniqueCount="789">
   <si>
     <t>https://uri.fiware.org/ns/data-models#status</t>
   </si>
@@ -2389,6 +2389,15 @@
   </si>
   <si>
     <t>FarmAnimal</t>
+  </si>
+  <si>
+    <t>typeName</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/ssn/Property</t>
+  </si>
+  <si>
+    <t>ssn.Property</t>
   </si>
 </sst>
 </file>
@@ -2775,10 +2784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15197C61-0C48-7940-A8EE-8D641CF5F3DB}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3096,6 +3105,14 @@
         <v>766</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>787</v>
+      </c>
+      <c r="C17" t="s">
+        <v>788</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3103,10 +3120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4A8733-A83C-1044-A18C-1ED63564F848}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3356,6 +3373,14 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>184</v>
+      </c>
+      <c r="C16" t="s">
+        <v>786</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>